<commit_message>
Actualizando casos de prueba y reportes de defectos para Sprint 2
</commit_message>
<xml_diff>
--- a/casosDePruebaYReporteDeDefectos.xlsx
+++ b/casosDePruebaYReporteDeDefectos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TECH-DEVELOPER\TRACK2_ESPECIALIZACION_FRONT\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B532899-70C4-4553-8B9D-B7BFCAFA35A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B7510B-1773-4A01-9227-617674728FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="105">
   <si>
     <t>Título</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>Regresión</t>
-  </si>
-  <si>
-    <t>TC-005</t>
   </si>
   <si>
     <t>Validar contraseña</t>
@@ -248,6 +245,105 @@
   </si>
   <si>
     <t>Se renderiza una notificación de éxito.</t>
+  </si>
+  <si>
+    <t>Click en el nombre del usuario redirige al Dashboard.</t>
+  </si>
+  <si>
+    <t>TC-006</t>
+  </si>
+  <si>
+    <t>Verificar que al hacer clic en el nombre del usuario, que se encuentra en el navbar, se redirige a la pantalla de Dashboard.</t>
+  </si>
+  <si>
+    <t>El usuario debe estar logueado en la aplicación.</t>
+  </si>
+  <si>
+    <t>Usuario autenticado en el sistema.</t>
+  </si>
+  <si>
+    <t>El sistema debe redirigir al usuario a la pantalla de Dashboard.</t>
+  </si>
+  <si>
+    <t>TC-005+A1A14:K18+A14:I16</t>
+  </si>
+  <si>
+    <t>1_Iniciar sesión en la aplicación.                    2_Dirigirte hacia algunas de las páginas del menú lateral, "Tu perfil", "Tarjetas", etc.  3_Hacer clic en el nombre del usuario en el navbar.</t>
+  </si>
+  <si>
+    <t>TC-007</t>
+  </si>
+  <si>
+    <t>Smoke.</t>
+  </si>
+  <si>
+    <t>1_Iniciar sesión en la aplicación.                      2_Navegar entre páginas del sistema.</t>
+  </si>
+  <si>
+    <t>La barra lateral debe permanecer visible en todas las páginas.</t>
+  </si>
+  <si>
+    <t>La barra lateral permanece visible en todas las páginas.</t>
+  </si>
+  <si>
+    <t>El sistema redirige al usuario a la pantalla de Dashboard.</t>
+  </si>
+  <si>
+    <t>TC-008</t>
+  </si>
+  <si>
+    <t>Nueva tarjeta</t>
+  </si>
+  <si>
+    <t>La barra lateral visible en todas las páginas.</t>
+  </si>
+  <si>
+    <t>Verificar que la barra lateral se mantenga visible en todas las páginas de la aplicación, si el usuario está logueado.</t>
+  </si>
+  <si>
+    <t>Verificar que al hacer clic en 'Nueva tarjeta' se redirige a la pantalla de alta de tarjeta.</t>
+  </si>
+  <si>
+    <t>El usuario debe estar logueado en la aplicación y debe tener acceso a la página de tarjetas.</t>
+  </si>
+  <si>
+    <t>1_Iniciar sesión en la aplicación.                      2_ Hacer click en "Tarjetas" del menú lateral.                                                                         3_Hacer click en "Nueva tarjeta"</t>
+  </si>
+  <si>
+    <t>Usuario autenticado.</t>
+  </si>
+  <si>
+    <t>El sistema debe redirigir a la pantalla de alta de tarjeta.</t>
+  </si>
+  <si>
+    <t>El sistema redirige a la pantalla de alta de tarjeta.</t>
+  </si>
+  <si>
+    <t>Máximo de 10 tarjetas, mostrar mensaje al llegar al límite.</t>
+  </si>
+  <si>
+    <t>TC-009</t>
+  </si>
+  <si>
+    <t>Verificar que al intentar agregar una tarjeta cuando ya hay 10, se muestre un mensaje de límite alcanzado.</t>
+  </si>
+  <si>
+    <t>El usuario debe estar logueado y debe haber agregado 10 tarjetas previamente.</t>
+  </si>
+  <si>
+    <t>1_Iniciar sesión en la aplicación.                      2_Asegurarse de que ya haya 10 tarjetas.     3_Intentar agregar la tarjeta número 11.</t>
+  </si>
+  <si>
+    <t>Usuario autenticado y con 10 tarjetas agregadas previamente.</t>
+  </si>
+  <si>
+    <t>El sistema debe mostrar un mensaje que indica que se ha alcanzado el límite de tarjetas (máximo 10).</t>
+  </si>
+  <si>
+    <t>El sistema muestra un mensaje que indica que se ha alcanzado el límite máximo de tarjetas.</t>
+  </si>
+  <si>
+    <t>Regresión.</t>
   </si>
 </sst>
 </file>
@@ -368,7 +464,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -389,14 +485,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -404,8 +500,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -691,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,19 +810,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -756,12 +855,12 @@
       <c r="J2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="4" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -789,12 +888,12 @@
         <v>50</v>
       </c>
       <c r="J3" s="7"/>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -806,10 +905,10 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="8"/>
+      <c r="K4" s="10"/>
     </row>
     <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -821,10 +920,10 @@
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
+      <c r="K5" s="10"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -836,10 +935,10 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-      <c r="K6" s="8"/>
+      <c r="K6" s="10"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -851,10 +950,10 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="8"/>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -884,12 +983,12 @@
       <c r="J8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K8" s="10" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -901,10 +1000,10 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="8"/>
+      <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -916,10 +1015,10 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="8"/>
+      <c r="K10" s="10"/>
     </row>
     <row r="11" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -931,7 +1030,7 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="8"/>
+      <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1001,28 +1100,28 @@
     </row>
     <row r="14" spans="1:11" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="H14" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>50</v>
@@ -1032,60 +1131,143 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+    <row r="15" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="K15" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="K16" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
-    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+    <row r="18" spans="1:11" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
+      <c r="K18" s="3" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="H3:H7"/>
     <mergeCell ref="J3:J7"/>
     <mergeCell ref="J8:J11"/>
     <mergeCell ref="A1:K1"/>
@@ -1102,11 +1284,6 @@
     <mergeCell ref="G8:G11"/>
     <mergeCell ref="H8:H11"/>
     <mergeCell ref="I8:I11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="H3:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>